<commit_message>
comparing new vs. old proposals
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_v3.xlsx
+++ b/app/data/wto_proposal_settings_master_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9791AEFC-034F-C54B-92DF-11F50DF5A577}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6F4C55-A885-7440-A959-5D217839BBD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="473">
   <si>
     <t>proposal</t>
   </si>
@@ -1264,9 +1264,6 @@
     <t>Chair's text - Consolidated text (June 2021) [Full exemption]</t>
   </si>
   <si>
-    <t>Chair's text - Consolidated text (June 2021) [Sustainability scenario]</t>
-  </si>
-  <si>
     <t>TN/RL/W/276/Rev.1 | Full exemption</t>
   </si>
   <si>
@@ -1372,9 +1369,6 @@
     <t>JUNE Chair's text - higher impact version (only manged get sustainabiliyt exemption, but we assume the high seas OFOC prohibition still applies to all)</t>
   </si>
   <si>
-    <t>JUNE Chair's text - sustainability criteria</t>
-  </si>
-  <si>
     <t xml:space="preserve">12/8/21 - Removed mistaken developing exemption for OFOC. 10/22/21 - Updated text. 7/13/21 - Updated text again. 6/8/21 - Updated text. 5/25/21 - NEW. </t>
   </si>
   <si>
@@ -1412,6 +1406,39 @@
   </si>
   <si>
     <t>1/5/22 - S&amp;DT for developing fixed for OFOC (capture production). 12/8/21 - Added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/21/22 - Added </t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs and developing countries shall be allowed. As written, such an exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text [Sustainability scenario]</t>
+  </si>
+  <si>
+    <t>JUNE/NOVEMBMER Chair's text - sustainability criteria</t>
+  </si>
+  <si>
+    <t>TN/RL/W/276/Rev.1 | Full exemption w/S&amp;DT error</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text (June 2021) [Full exemption w/S&amp;DT error]</t>
+  </si>
+  <si>
+    <t>JUNE Chair's text - old low end version (everyone gets sustainability exemption and we assume the high seas OFOC prohibition only applies to developed)</t>
+  </si>
+  <si>
+    <t>JUNE/NOVEMBMER Chair's text - sustainability criteria old version</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text [Sustainability scenario w/S&amp;DT error]</t>
+  </si>
+  <si>
+    <t>TN/RL/W/276/Rev.1 | Sustainability scenario w/S&amp;DT error</t>
+  </si>
+  <si>
+    <t>Subsidies granted by developing and LDC Members shall be allowed. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
   </si>
 </sst>
 </file>
@@ -2381,11 +2408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CW47"/>
+  <dimension ref="A1:CW49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="BR45" sqref="BR45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2728,7 +2755,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>325</v>
@@ -4178,7 +4205,7 @@
         <v>174</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G20" s="10">
         <v>43803</v>
@@ -4255,7 +4282,7 @@
         <v>174</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G21" s="10">
         <v>43803</v>
@@ -4709,7 +4736,7 @@
         <v>38</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>294</v>
@@ -4733,7 +4760,7 @@
         <v>374</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="S26" s="24" t="s">
         <v>38</v>
@@ -4884,7 +4911,7 @@
         <v>298</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>110</v>
@@ -4926,7 +4953,7 @@
         <v>374</v>
       </c>
       <c r="R27" s="23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S27" s="23" t="s">
         <v>38</v>
@@ -5017,7 +5044,7 @@
         <v>160</v>
       </c>
       <c r="BS27" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV27" s="9" t="s">
         <v>153</v>
@@ -5117,7 +5144,7 @@
         <v>382</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>196</v>
@@ -5165,7 +5192,7 @@
         <v>239</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>196</v>
@@ -5207,7 +5234,7 @@
         <v>386</v>
       </c>
       <c r="R30" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S30" s="23" t="s">
         <v>38</v>
@@ -5291,7 +5318,7 @@
         <v>160</v>
       </c>
       <c r="BS30" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV30" s="9" t="s">
         <v>153</v>
@@ -5311,7 +5338,7 @@
         <v>238</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>196</v>
@@ -5353,7 +5380,7 @@
         <v>386</v>
       </c>
       <c r="R31" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S31" s="23" t="s">
         <v>38</v>
@@ -5437,7 +5464,7 @@
         <v>160</v>
       </c>
       <c r="BS31" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV31" s="9" t="s">
         <v>153</v>
@@ -5457,7 +5484,7 @@
         <v>234</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>196</v>
@@ -5499,7 +5526,7 @@
         <v>386</v>
       </c>
       <c r="R32" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S32" s="23" t="s">
         <v>344</v>
@@ -5583,7 +5610,7 @@
         <v>160</v>
       </c>
       <c r="BS32" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV32" s="9" t="s">
         <v>153</v>
@@ -5610,7 +5637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>221</v>
       </c>
@@ -5621,7 +5648,7 @@
         <v>235</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>196</v>
@@ -5663,7 +5690,7 @@
         <v>386</v>
       </c>
       <c r="R33" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S33" s="23" t="s">
         <v>344</v>
@@ -5747,7 +5774,7 @@
         <v>160</v>
       </c>
       <c r="BS33" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV33" s="9" t="s">
         <v>153</v>
@@ -5774,7 +5801,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>221</v>
       </c>
@@ -5785,7 +5812,7 @@
         <v>232</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>196</v>
@@ -5827,7 +5854,7 @@
         <v>386</v>
       </c>
       <c r="R34" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S34" s="23" t="s">
         <v>345</v>
@@ -5896,7 +5923,7 @@
         <v>160</v>
       </c>
       <c r="BS34" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV34" s="9" t="s">
         <v>153</v>
@@ -5932,7 +5959,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>221</v>
       </c>
@@ -5943,7 +5970,7 @@
         <v>233</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>196</v>
@@ -5985,7 +6012,7 @@
         <v>386</v>
       </c>
       <c r="R35" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S35" s="23" t="s">
         <v>345</v>
@@ -6054,7 +6081,7 @@
         <v>160</v>
       </c>
       <c r="BS35" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV35" s="9" t="s">
         <v>153</v>
@@ -6090,7 +6117,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>221</v>
       </c>
@@ -6101,7 +6128,7 @@
         <v>231</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>196</v>
@@ -6143,7 +6170,7 @@
         <v>386</v>
       </c>
       <c r="R36" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S36" s="23" t="s">
         <v>324</v>
@@ -6212,7 +6239,7 @@
         <v>160</v>
       </c>
       <c r="BS36" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV36" s="9" t="s">
         <v>153</v>
@@ -6249,7 +6276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>221</v>
       </c>
@@ -6260,7 +6287,7 @@
         <v>230</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>196</v>
@@ -6302,7 +6329,7 @@
         <v>386</v>
       </c>
       <c r="R37" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S37" s="23" t="s">
         <v>324</v>
@@ -6371,7 +6398,7 @@
         <v>160</v>
       </c>
       <c r="BS37" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV37" s="9" t="s">
         <v>153</v>
@@ -6408,7 +6435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:101" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:98" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>221</v>
       </c>
@@ -6419,7 +6446,7 @@
         <v>228</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>196</v>
@@ -6461,7 +6488,7 @@
         <v>386</v>
       </c>
       <c r="R38" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S38" s="24" t="s">
         <v>371</v>
@@ -6530,7 +6557,7 @@
         <v>160</v>
       </c>
       <c r="BS38" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV38" s="9" t="s">
         <v>153</v>
@@ -6548,7 +6575,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>221</v>
       </c>
@@ -6559,7 +6586,7 @@
         <v>229</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>196</v>
@@ -6601,7 +6628,7 @@
         <v>386</v>
       </c>
       <c r="R39" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S39" s="24" t="s">
         <v>371</v>
@@ -6670,7 +6697,7 @@
         <v>160</v>
       </c>
       <c r="BS39" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV39" s="9" t="s">
         <v>153</v>
@@ -6688,7 +6715,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
@@ -6697,7 +6724,7 @@
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>282</v>
@@ -6733,7 +6760,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="41" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
@@ -6744,7 +6771,7 @@
         <v>305</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>286</v>
@@ -6762,7 +6789,7 @@
         <v>38</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>285</v>
@@ -6786,7 +6813,7 @@
         <v>386</v>
       </c>
       <c r="R41" s="23" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S41" s="23" t="s">
         <v>38</v>
@@ -6864,7 +6891,7 @@
         <v>160</v>
       </c>
       <c r="BS41" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV41" s="9" t="s">
         <v>153</v>
@@ -6873,7 +6900,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>39</v>
       </c>
@@ -6881,22 +6908,22 @@
         <v>351</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>413</v>
+        <v>467</v>
       </c>
       <c r="G42" s="10">
         <v>44327</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>415</v>
+        <v>466</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>39</v>
@@ -6914,19 +6941,19 @@
         <v>410</v>
       </c>
       <c r="N42" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O42" s="23" t="s">
         <v>411</v>
       </c>
       <c r="P42" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q42" s="23" t="s">
         <v>412</v>
       </c>
       <c r="R42" s="23" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="S42" s="23" t="s">
         <v>38</v>
@@ -7010,7 +7037,7 @@
         <v>160</v>
       </c>
       <c r="BS42" s="9" t="s">
-        <v>453</v>
+        <v>152</v>
       </c>
       <c r="BV42" s="9" t="s">
         <v>153</v>
@@ -7019,7 +7046,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
@@ -7030,19 +7057,19 @@
         <v>450</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G43" s="10">
         <v>44327</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>321</v>
+        <v>414</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>39</v>
@@ -7051,28 +7078,28 @@
         <v>195</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>416</v>
+        <v>320</v>
       </c>
       <c r="L43" s="9" t="s">
         <v>307</v>
       </c>
       <c r="M43" s="23" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="N43" s="23" t="s">
-        <v>250</v>
+        <v>424</v>
       </c>
       <c r="O43" s="23" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="P43" s="23" t="s">
-        <v>250</v>
+        <v>425</v>
       </c>
       <c r="Q43" s="23" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="R43" s="23" t="s">
-        <v>426</v>
+        <v>444</v>
       </c>
       <c r="S43" s="23" t="s">
         <v>38</v>
@@ -7081,28 +7108,31 @@
         <v>306</v>
       </c>
       <c r="U43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="V43" s="9">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="W43" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Z43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="AA43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="AB43" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AD43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="AE43" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AG43" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AJ43" s="9" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="AK43" s="9" t="s">
         <v>191</v>
@@ -7111,13 +7141,19 @@
         <v>152</v>
       </c>
       <c r="AR43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="AS43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="AT43" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AW43" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="AX43" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="BA43" s="9" t="s">
         <v>153</v>
@@ -7129,22 +7165,25 @@
         <v>191</v>
       </c>
       <c r="BG43" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI43" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BO43" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="BM43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="BN43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="BO43" s="9" t="s">
-        <v>198</v>
-      </c>
       <c r="BR43" s="9" t="s">
         <v>160</v>
       </c>
       <c r="BS43" s="9" t="s">
-        <v>198</v>
+        <v>451</v>
       </c>
       <c r="BV43" s="9" t="s">
         <v>153</v>
@@ -7153,7 +7192,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>39</v>
       </c>
@@ -7161,22 +7200,22 @@
         <v>351</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G44" s="10">
         <v>44327</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>39</v>
@@ -7185,7 +7224,7 @@
         <v>195</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L44" s="9" t="s">
         <v>307</v>
@@ -7194,19 +7233,19 @@
         <v>410</v>
       </c>
       <c r="N44" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O44" s="23" t="s">
         <v>411</v>
       </c>
       <c r="P44" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R44" s="23" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="S44" s="23" t="s">
         <v>38</v>
@@ -7272,7 +7311,7 @@
         <v>191</v>
       </c>
       <c r="BG44" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="BI44" s="9">
         <v>5</v>
@@ -7290,7 +7329,7 @@
         <v>160</v>
       </c>
       <c r="BS44" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BV44" s="9" t="s">
         <v>153</v>
@@ -7299,7 +7338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>39</v>
       </c>
@@ -7307,52 +7346,52 @@
         <v>351</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>439</v>
+        <v>469</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>432</v>
+        <v>196</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>433</v>
+        <v>470</v>
       </c>
       <c r="G45" s="10">
-        <v>44524</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>443</v>
+        <v>44327</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>471</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>435</v>
+        <v>195</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>436</v>
+        <v>307</v>
       </c>
       <c r="M45" s="23" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="N45" s="23" t="s">
-        <v>437</v>
+        <v>250</v>
       </c>
       <c r="O45" s="23" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="P45" s="23" t="s">
-        <v>437</v>
+        <v>250</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="R45" s="23" t="s">
-        <v>444</v>
+        <v>472</v>
       </c>
       <c r="S45" s="23" t="s">
         <v>38</v>
@@ -7361,31 +7400,28 @@
         <v>306</v>
       </c>
       <c r="U45" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="V45" s="9">
+        <v>20</v>
       </c>
       <c r="W45" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Z45" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AA45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB45" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AD45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE45" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AG45" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AJ45" s="9" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="AK45" s="9" t="s">
         <v>191</v>
@@ -7394,19 +7430,13 @@
         <v>152</v>
       </c>
       <c r="AR45" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AS45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT45" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AW45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AX45" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="BA45" s="9" t="s">
         <v>153</v>
@@ -7418,10 +7448,7 @@
         <v>191</v>
       </c>
       <c r="BG45" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="BI45" s="9">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="BM45" s="9" t="s">
         <v>160</v>
@@ -7430,14 +7457,14 @@
         <v>160</v>
       </c>
       <c r="BO45" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="BR45" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BS45" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="BR45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="BS45" s="9" t="s">
-        <v>454</v>
-      </c>
       <c r="BV45" s="9" t="s">
         <v>153</v>
       </c>
@@ -7445,7 +7472,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>39</v>
       </c>
@@ -7453,52 +7480,52 @@
         <v>351</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>440</v>
+        <v>465</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>432</v>
+        <v>196</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="G46" s="10">
-        <v>44524</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>442</v>
+        <v>44327</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>321</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>435</v>
+        <v>195</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>436</v>
+        <v>307</v>
       </c>
       <c r="M46" s="23" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="N46" s="23" t="s">
-        <v>437</v>
+        <v>250</v>
       </c>
       <c r="O46" s="23" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="P46" s="23" t="s">
-        <v>437</v>
+        <v>250</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="R46" s="23" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="S46" s="23" t="s">
         <v>38</v>
@@ -7507,31 +7534,28 @@
         <v>306</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
+      </c>
+      <c r="V46" s="9">
+        <v>20</v>
       </c>
       <c r="W46" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Z46" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AA46" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB46" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AD46" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE46" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AG46" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AJ46" s="9" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="AK46" s="9" t="s">
         <v>191</v>
@@ -7540,19 +7564,13 @@
         <v>152</v>
       </c>
       <c r="AR46" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AS46" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT46" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="AW46" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AX46" s="9" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="BA46" s="9" t="s">
         <v>153</v>
@@ -7564,10 +7582,7 @@
         <v>191</v>
       </c>
       <c r="BG46" s="9" t="s">
-        <v>431</v>
-      </c>
-      <c r="BI46" s="9">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="BM46" s="9" t="s">
         <v>160</v>
@@ -7576,13 +7591,13 @@
         <v>160</v>
       </c>
       <c r="BO46" s="9" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="BR46" s="9" t="s">
         <v>160</v>
       </c>
       <c r="BS46" s="9" t="s">
-        <v>454</v>
+        <v>198</v>
       </c>
       <c r="BV46" s="9" t="s">
         <v>153</v>
@@ -7591,212 +7606,504 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:101" ht="42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="20"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="H47" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I47" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="G47" s="10">
+        <v>44524</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="I47" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="J47" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="M47" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="N47" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="O47" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="P47" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q47" s="23" t="s">
+        <v>412</v>
+      </c>
+      <c r="R47" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="S47" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T47" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="U47" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="V47" s="9">
-        <v>20</v>
       </c>
       <c r="W47" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Z47" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="AA47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC47" s="9">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="AB47" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AD47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AF47" s="9">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="AE47" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AG47" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AI47" s="9">
-        <v>5</v>
+      <c r="AJ47" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK47" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="AL47" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="AN47" s="9">
-        <v>5</v>
-      </c>
-      <c r="AO47" s="9">
-        <v>24</v>
-      </c>
-      <c r="AP47" s="9">
-        <v>100</v>
-      </c>
-      <c r="AQ47" s="9">
-        <v>400</v>
-      </c>
       <c r="AR47" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="AS47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AU47" s="9">
-        <v>5</v>
-      </c>
-      <c r="AV47" s="9">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="AT47" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="AW47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AY47" s="9">
-        <v>5</v>
-      </c>
-      <c r="AZ47" s="9">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="AX47" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="BA47" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="BC47" s="9">
-        <v>5</v>
-      </c>
-      <c r="BD47" s="9">
-        <v>5</v>
+      <c r="BE47" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="BF47" s="9" t="s">
-        <v>152</v>
+        <v>191</v>
+      </c>
+      <c r="BG47" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="BI47" s="9">
         <v>5</v>
       </c>
-      <c r="BJ47" s="9">
+      <c r="BM47" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN47" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BO47" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="BR47" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BS47" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="BV47" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ47" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:98" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G48" s="10">
+        <v>44524</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="M48" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="N48" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="O48" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="P48" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q48" s="23" t="s">
+        <v>422</v>
+      </c>
+      <c r="R48" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="S48" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T48" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="U48" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="W48" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB48" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE48" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG48" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ48" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK48" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL48" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AR48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT48" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AX48" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="BA48" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BE48" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="BF48" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="BG48" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="BI48" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BO48" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="BR48" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BS48" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="BV48" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ48" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:101" ht="42" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="20"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="H49" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="U49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="V49" s="9">
+        <v>20</v>
+      </c>
+      <c r="W49" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC49" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF49" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI49" s="9">
+        <v>5</v>
+      </c>
+      <c r="AL49" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN49" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO49" s="9">
         <v>24</v>
       </c>
-      <c r="BK47" s="9">
+      <c r="AP49" s="9">
         <v>100</v>
       </c>
-      <c r="BL47" s="9">
+      <c r="AQ49" s="9">
         <v>400</v>
       </c>
-      <c r="BM47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="BN47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="BP47" s="9">
+      <c r="AR49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU49" s="9">
         <v>5</v>
       </c>
-      <c r="BQ47" s="9">
+      <c r="AV49" s="9">
         <v>5</v>
       </c>
-      <c r="BR47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="BT47" s="9">
+      <c r="AW49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY49" s="9">
         <v>5</v>
       </c>
-      <c r="BU47" s="9">
+      <c r="AZ49" s="9">
         <v>5</v>
       </c>
-      <c r="BV47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="BX47" s="9">
+      <c r="BA49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC49" s="9">
         <v>5</v>
       </c>
-      <c r="BY47" s="9">
+      <c r="BD49" s="9">
         <v>5</v>
       </c>
-      <c r="BZ47" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="CA47" s="9" t="s">
+      <c r="BF49" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="BI49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ49" s="9">
+        <v>24</v>
+      </c>
+      <c r="BK49" s="9">
+        <v>100</v>
+      </c>
+      <c r="BL49" s="9">
+        <v>400</v>
+      </c>
+      <c r="BM49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BP49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BQ49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BR49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BU49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BV49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BX49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BY49" s="9">
+        <v>5</v>
+      </c>
+      <c r="BZ49" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="CA49" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="CB47" s="9" t="s">
+      <c r="CB49" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="CC47" s="9" t="s">
+      <c r="CC49" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="CD47" s="9">
+      <c r="CD49" s="9">
         <v>0.7</v>
       </c>
-      <c r="CE47" s="9" t="s">
+      <c r="CE49" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="CF47" s="9" t="s">
+      <c r="CF49" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="CG47" s="9">
+      <c r="CG49" s="9">
         <v>50</v>
       </c>
-      <c r="CH47" s="16">
+      <c r="CH49" s="16">
         <v>5</v>
       </c>
-      <c r="CI47" s="16">
+      <c r="CI49" s="16">
         <v>5</v>
       </c>
-      <c r="CJ47" s="16">
+      <c r="CJ49" s="16">
         <v>5</v>
       </c>
-      <c r="CK47" s="16">
+      <c r="CK49" s="16">
         <v>5</v>
       </c>
-      <c r="CL47" s="9" t="s">
+      <c r="CL49" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="CM47" s="9">
+      <c r="CM49" s="9">
         <v>5</v>
       </c>
-      <c r="CN47" s="9">
+      <c r="CN49" s="9">
         <v>5</v>
       </c>
-      <c r="CO47" s="16">
+      <c r="CO49" s="16">
         <v>5</v>
       </c>
-      <c r="CP47" s="16">
+      <c r="CP49" s="16">
         <v>5</v>
       </c>
-      <c r="CQ47" s="16">
+      <c r="CQ49" s="16">
         <v>5</v>
       </c>
-      <c r="CR47" s="9" t="s">
+      <c r="CR49" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="CS47" s="9">
+      <c r="CS49" s="9">
         <v>5</v>
       </c>
-      <c r="CT47" s="9">
+      <c r="CT49" s="9">
         <v>5</v>
       </c>
-      <c r="CU47" s="16">
+      <c r="CU49" s="16">
         <v>5</v>
       </c>
-      <c r="CV47" s="16">
+      <c r="CV49" s="16">
         <v>5</v>
       </c>
-      <c r="CW47" s="16">
+      <c r="CW49" s="16">
         <v>5</v>
       </c>
     </row>

</xml_diff>